<commit_message>
Fri, Oct 23, 2020 10:08:58 AM
</commit_message>
<xml_diff>
--- a/Data/Summary - Peak Velocity.xlsx
+++ b/Data/Summary - Peak Velocity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groberts\Documents\MCH Ischemia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groberts\Documents\Research Projects\MCH_Ischemia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Negative Diagnosis" sheetId="3" r:id="rId1"/>
@@ -17,8 +17,7 @@
     <sheet name="Ischemia" sheetId="5" r:id="rId3"/>
     <sheet name="Unknown" sheetId="6" r:id="rId4"/>
     <sheet name="Controls" sheetId="7" r:id="rId5"/>
-    <sheet name="..." sheetId="8" r:id="rId6"/>
-    <sheet name="T-test" sheetId="9" r:id="rId7"/>
+    <sheet name="T-test" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1594,6 +1593,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="39" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1610,15 +1618,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9894,7 +9893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
@@ -10073,7 +10072,7 @@
       <c r="A5" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="142" t="s">
         <v>88</v>
       </c>
       <c r="C5" s="20">
@@ -10112,7 +10111,7 @@
       <c r="A6" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="140"/>
+      <c r="B6" s="143"/>
       <c r="C6" s="20">
         <v>88.811700000000002</v>
       </c>
@@ -10149,7 +10148,7 @@
       <c r="A7" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="141"/>
+      <c r="B7" s="144"/>
       <c r="C7" s="7">
         <f>(C6-C5)/C5*100</f>
         <v>2.7783531938679076</v>
@@ -10660,7 +10659,7 @@
       <c r="A20" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="143" t="s">
         <v>100</v>
       </c>
       <c r="C20" s="7">
@@ -10700,7 +10699,7 @@
       <c r="A21" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="140"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="7">
         <v>85.280600000000007</v>
       </c>
@@ -10752,7 +10751,7 @@
       <c r="A22" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="142"/>
+      <c r="B22" s="145"/>
       <c r="C22" s="7">
         <f>(C21-C20)/C20*100</f>
         <v>-6.1117227408842556</v>
@@ -11121,7 +11120,7 @@
       <c r="A32" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="143" t="s">
+      <c r="B32" s="146" t="s">
         <v>114</v>
       </c>
       <c r="C32" s="7">
@@ -11156,7 +11155,7 @@
       <c r="A33" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B33" s="143"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="7">
         <v>89.401799999999994</v>
       </c>
@@ -11190,7 +11189,7 @@
       <c r="A34" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="144"/>
+      <c r="B34" s="147"/>
       <c r="C34" s="7">
         <f>(C33-C32)/C32*100</f>
         <v>10.024182680770144</v>
@@ -12356,7 +12355,7 @@
       <c r="A65" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="B65" s="145" t="s">
+      <c r="B65" s="139" t="s">
         <v>141</v>
       </c>
       <c r="C65" s="25">
@@ -12392,7 +12391,7 @@
       <c r="A66" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B66" s="146"/>
+      <c r="B66" s="140"/>
       <c r="C66" s="20">
         <v>121.3188</v>
       </c>
@@ -12426,7 +12425,7 @@
       <c r="A67" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="147"/>
+      <c r="B67" s="141"/>
       <c r="C67" s="4">
         <f>(C66-C65)/C65*100</f>
         <v>-5.421700835870892</v>
@@ -12759,16 +12758,16 @@
     <row r="108" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B32:B34"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="B65:B67"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B32:B34"/>
   </mergeCells>
   <conditionalFormatting sqref="M21:M22 O21:AC21 AA20">
     <cfRule type="colorScale" priority="75">
@@ -13100,24 +13099,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ99"/>
   <sheetViews>
-    <sheetView topLeftCell="L58" workbookViewId="0">
-      <selection activeCell="AA106" sqref="M104:AA106"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>